<commit_message>
Fixes, adding more libs, restructured dirs
</commit_message>
<xml_diff>
--- a/Game engines with source.xlsx
+++ b/Game engines with source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Abstractorizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9131161D-710F-48BC-9183-CE10AB058755}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D54060-BC02-433C-9A9C-2BA980346AB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D89808C4-C9D4-43AC-AFF6-65FCC2C0AB98}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="303">
   <si>
     <t xml:space="preserve">The Freeciv Project </t>
   </si>
@@ -927,6 +927,24 @@
   </si>
   <si>
     <t>C++/Python</t>
+  </si>
+  <si>
+    <t>https://github.com/Angelo1211/HybridRenderingEngine</t>
+  </si>
+  <si>
+    <t>Hybrid Rendering Engine</t>
+  </si>
+  <si>
+    <t>https://github.com/xelatihy/yocto-gl</t>
+  </si>
+  <si>
+    <t>Yocto-gl</t>
+  </si>
+  <si>
+    <t>https://github.com/Nadrin/PBR</t>
+  </si>
+  <si>
+    <t>PBR</t>
   </si>
 </sst>
 </file>
@@ -1407,10 +1425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84666BE2-700C-4D0F-8E71-7A46C3A604FB}">
-  <dimension ref="A1:L94"/>
+  <dimension ref="A1:L98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2039,495 +2057,495 @@
       </c>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" t="s">
-        <v>287</v>
-      </c>
       <c r="B40" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="H40" t="s">
-        <v>34</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J40" t="s">
-        <v>31</v>
+        <v>216</v>
       </c>
       <c r="K40" s="3"/>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" t="s">
-        <v>291</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>90</v>
+        <v>287</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>286</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
+        <v>34</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J41" t="s">
+        <v>31</v>
+      </c>
+      <c r="K41" s="3"/>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" t="s">
+        <v>291</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G42" t="s">
         <v>295</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H42" t="s">
         <v>82</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J42" t="s">
         <v>89</v>
       </c>
-      <c r="K41" s="3" t="s">
+      <c r="K42" s="3" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="5" customFormat="1">
-      <c r="A42" s="5" t="s">
+    <row r="43" spans="1:11" s="5" customFormat="1">
+      <c r="A43" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="I42" s="20" t="s">
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="I43" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="J42" s="5" t="s">
+      <c r="J43" s="5" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
-      <c r="B43" s="3" t="s">
+    <row r="44" spans="1:11">
+      <c r="B44" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C44" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H44" t="s">
         <v>34</v>
       </c>
-      <c r="I43" s="9" t="s">
+      <c r="I44" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="J43" t="s">
+      <c r="J44" t="s">
         <v>120</v>
       </c>
-      <c r="K43" s="8" t="s">
+      <c r="K44" s="8" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
-      <c r="A44" t="s">
+    <row r="45" spans="1:11">
+      <c r="A45" t="s">
         <v>284</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C45" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H45" t="s">
         <v>37</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="I45" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J45" t="s">
         <v>30</v>
       </c>
-      <c r="K44" s="3" t="s">
+      <c r="K45" s="3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
-      <c r="B45" s="12" t="s">
+    <row r="46" spans="1:11">
+      <c r="B46" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="C45" s="12"/>
-      <c r="G45" t="s">
+      <c r="C46" s="12"/>
+      <c r="G46" t="s">
         <v>136</v>
       </c>
-      <c r="J45" s="10" t="s">
+      <c r="J46" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="K45" s="11"/>
-    </row>
-    <row r="46" spans="1:11">
-      <c r="B46" t="s">
+      <c r="K46" s="11"/>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="B47" t="s">
         <v>48</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C47" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D46" s="20" t="s">
+      <c r="D47" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="H47" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J47" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11">
-      <c r="B47" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="H47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J47" t="s">
-        <v>33</v>
-      </c>
-      <c r="K47" s="3" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="48" spans="1:11">
       <c r="B48" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="H48" t="s">
+        <v>34</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J48" t="s">
+        <v>33</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="B49" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H48" s="3" t="s">
+      <c r="H49" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J48" t="s">
+      <c r="J49" t="s">
         <v>118</v>
-      </c>
-      <c r="K48" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12">
-      <c r="B49" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G49" t="s">
-        <v>61</v>
-      </c>
-      <c r="H49" t="s">
-        <v>34</v>
-      </c>
-      <c r="J49" t="s">
-        <v>60</v>
       </c>
       <c r="K49" t="s">
         <v>128</v>
       </c>
-      <c r="L49" t="s">
+    </row>
+    <row r="50" spans="1:12">
+      <c r="B50" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G50" t="s">
+        <v>61</v>
+      </c>
+      <c r="H50" t="s">
+        <v>34</v>
+      </c>
+      <c r="J50" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="50" spans="1:12">
-      <c r="B50" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H50" t="s">
-        <v>121</v>
-      </c>
-      <c r="J50" t="s">
-        <v>27</v>
-      </c>
       <c r="K50" t="s">
-        <v>26</v>
+        <v>128</v>
+      </c>
+      <c r="L50" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:12">
       <c r="B51" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H51" t="s">
+        <v>121</v>
+      </c>
+      <c r="J51" t="s">
+        <v>27</v>
+      </c>
+      <c r="K51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="B52" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="G51" s="8" t="s">
+      <c r="G52" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="J51" t="s">
+      <c r="J52" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
-      <c r="B52" s="5" t="s">
+    <row r="53" spans="1:12">
+      <c r="B53" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="J52" t="s">
+      <c r="J53" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
-      <c r="B53" t="s">
+    <row r="54" spans="1:12">
+      <c r="B54" t="s">
         <v>239</v>
       </c>
-      <c r="J53" t="s">
+      <c r="J54" t="s">
         <v>238</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12">
-      <c r="B54" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="G54" t="s">
-        <v>242</v>
-      </c>
-      <c r="J54" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="55" spans="1:12">
       <c r="B55" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="G55" t="s">
+        <v>242</v>
+      </c>
+      <c r="J55" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="B56" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C56" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G56" t="s">
         <v>290</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J56" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="56" spans="1:12" s="15" customFormat="1">
-      <c r="A56" s="15" t="s">
+    <row r="57" spans="1:12" s="15" customFormat="1">
+      <c r="A57" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="I56" s="16"/>
-    </row>
-    <row r="57" spans="1:12">
-      <c r="B57" s="5" t="s">
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
+      <c r="I57" s="16"/>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="B58" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="E57" s="23" t="s">
+      <c r="E58" s="23" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12">
-      <c r="A58" t="s">
-        <v>283</v>
-      </c>
-      <c r="B58" s="14" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" t="s">
+        <v>283</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" t="s">
         <v>251</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B60" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G60" t="s">
         <v>64</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H60" t="s">
         <v>82</v>
       </c>
-      <c r="J59" t="s">
+      <c r="J60" t="s">
         <v>63</v>
       </c>
-      <c r="K59" s="3" t="s">
+      <c r="K60" s="3" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="60" spans="1:12">
-      <c r="B60" s="19" t="s">
+    <row r="61" spans="1:12">
+      <c r="B61" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="H60" t="s">
+      <c r="H61" t="s">
         <v>37</v>
       </c>
-      <c r="I60" s="2" t="s">
+      <c r="I61" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J60" t="s">
+      <c r="J61" t="s">
         <v>43</v>
       </c>
-      <c r="K60" s="3" t="s">
+      <c r="K61" s="3" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12">
-      <c r="B61" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="G61" t="s">
-        <v>144</v>
-      </c>
-      <c r="H61" t="s">
-        <v>34</v>
-      </c>
-      <c r="J61" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="62" spans="1:12">
       <c r="B62" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="H62" t="s">
-        <v>37</v>
-      </c>
-      <c r="J62" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="K62" s="3" t="s">
-        <v>162</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="J62" t="s">
+        <v>299</v>
+      </c>
+      <c r="K62" s="3"/>
     </row>
     <row r="63" spans="1:12">
       <c r="B63" s="5" t="s">
-        <v>150</v>
+        <v>302</v>
+      </c>
+      <c r="J63" t="s">
+        <v>301</v>
       </c>
       <c r="K63" s="3"/>
     </row>
     <row r="64" spans="1:12">
       <c r="B64" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="J64" t="s">
+        <v>297</v>
+      </c>
+      <c r="K64" s="3"/>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="B65" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="G65" t="s">
+        <v>144</v>
+      </c>
+      <c r="H65" t="s">
+        <v>34</v>
+      </c>
+      <c r="J65" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="B66" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="H66" t="s">
+        <v>37</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K66" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="B67" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="K67" s="3"/>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="B68" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="K64" s="3"/>
-    </row>
-    <row r="65" spans="1:11">
-      <c r="B65" t="s">
-        <v>74</v>
-      </c>
-      <c r="G65" t="s">
-        <v>73</v>
-      </c>
-      <c r="H65" t="s">
-        <v>37</v>
-      </c>
-      <c r="J65" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11">
-      <c r="B66" t="s">
-        <v>115</v>
-      </c>
-      <c r="G66" t="s">
-        <v>116</v>
-      </c>
-      <c r="H66" t="s">
-        <v>34</v>
-      </c>
-      <c r="J66" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11">
-      <c r="B67" t="s">
-        <v>134</v>
-      </c>
-      <c r="G67" t="s">
-        <v>132</v>
-      </c>
-      <c r="H67" t="s">
-        <v>34</v>
-      </c>
-      <c r="J67" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11">
-      <c r="B68" t="s">
-        <v>79</v>
-      </c>
-      <c r="G68" t="s">
-        <v>78</v>
-      </c>
-      <c r="H68" t="s">
-        <v>34</v>
-      </c>
-      <c r="J68" t="s">
-        <v>77</v>
-      </c>
-      <c r="K68" t="s">
-        <v>26</v>
-      </c>
+      <c r="K68" s="3"/>
     </row>
     <row r="69" spans="1:11">
       <c r="B69" t="s">
-        <v>130</v>
+        <v>74</v>
       </c>
       <c r="G69" t="s">
-        <v>129</v>
+        <v>73</v>
       </c>
       <c r="H69" t="s">
-        <v>131</v>
+        <v>37</v>
       </c>
       <c r="J69" t="s">
-        <v>126</v>
-      </c>
-      <c r="K69" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:11">
+      <c r="B70" t="s">
+        <v>115</v>
+      </c>
+      <c r="G70" t="s">
+        <v>116</v>
+      </c>
+      <c r="H70" t="s">
+        <v>34</v>
+      </c>
       <c r="J70" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
     </row>
     <row r="71" spans="1:11">
       <c r="B71" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="G71" t="s">
-        <v>165</v>
+        <v>132</v>
+      </c>
+      <c r="H71" t="s">
+        <v>34</v>
       </c>
       <c r="J71" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" s="15" customFormat="1">
-      <c r="A72" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="D72" s="16"/>
-      <c r="E72" s="16"/>
-      <c r="F72" s="16"/>
-      <c r="I72" s="16"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="B72" t="s">
+        <v>79</v>
+      </c>
+      <c r="G72" t="s">
+        <v>78</v>
+      </c>
+      <c r="H72" t="s">
+        <v>34</v>
+      </c>
+      <c r="J72" t="s">
+        <v>77</v>
+      </c>
+      <c r="K72" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="73" spans="1:11">
       <c r="B73" t="s">
-        <v>182</v>
+        <v>130</v>
+      </c>
+      <c r="G73" t="s">
+        <v>129</v>
+      </c>
+      <c r="H73" t="s">
+        <v>131</v>
+      </c>
+      <c r="J73" t="s">
+        <v>126</v>
+      </c>
+      <c r="K73" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="74" spans="1:11">
-      <c r="B74" t="s">
-        <v>163</v>
-      </c>
-      <c r="G74" t="s">
-        <v>184</v>
-      </c>
-      <c r="K74" t="s">
-        <v>164</v>
+      <c r="J74" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:11">
       <c r="B75" t="s">
-        <v>124</v>
+        <v>167</v>
+      </c>
+      <c r="G75" t="s">
+        <v>165</v>
       </c>
       <c r="J75" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
     </row>
     <row r="76" spans="1:11" s="15" customFormat="1">
       <c r="A76" s="15" t="s">
-        <v>117</v>
+        <v>181</v>
       </c>
       <c r="D76" s="16"/>
       <c r="E76" s="16"/>
@@ -2536,49 +2554,31 @@
     </row>
     <row r="77" spans="1:11">
       <c r="B77" t="s">
-        <v>88</v>
-      </c>
-      <c r="G77" t="s">
-        <v>81</v>
-      </c>
-      <c r="H77" t="s">
-        <v>82</v>
-      </c>
-      <c r="J77" t="s">
-        <v>80</v>
+        <v>182</v>
       </c>
     </row>
     <row r="78" spans="1:11">
       <c r="B78" t="s">
-        <v>84</v>
+        <v>163</v>
       </c>
       <c r="G78" t="s">
-        <v>85</v>
-      </c>
-      <c r="H78" t="s">
-        <v>87</v>
-      </c>
-      <c r="J78" t="s">
-        <v>83</v>
+        <v>184</v>
+      </c>
+      <c r="K78" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="79" spans="1:11">
       <c r="B79" t="s">
-        <v>86</v>
-      </c>
-      <c r="G79" t="s">
-        <v>85</v>
-      </c>
-      <c r="H79" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
       <c r="J79" t="s">
-        <v>86</v>
+        <v>183</v>
       </c>
     </row>
     <row r="80" spans="1:11" s="15" customFormat="1">
       <c r="A80" s="15" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="D80" s="16"/>
       <c r="E80" s="16"/>
@@ -2587,124 +2587,175 @@
     </row>
     <row r="81" spans="1:10">
       <c r="B81" t="s">
-        <v>69</v>
+        <v>88</v>
+      </c>
+      <c r="G81" t="s">
+        <v>81</v>
+      </c>
+      <c r="H81" t="s">
+        <v>82</v>
       </c>
       <c r="J81" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
     </row>
     <row r="82" spans="1:10">
       <c r="B82" t="s">
-        <v>41</v>
+        <v>84</v>
+      </c>
+      <c r="G82" t="s">
+        <v>85</v>
+      </c>
+      <c r="H82" t="s">
+        <v>87</v>
       </c>
       <c r="J82" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
     </row>
     <row r="83" spans="1:10">
       <c r="B83" t="s">
-        <v>70</v>
+        <v>86</v>
+      </c>
+      <c r="G83" t="s">
+        <v>85</v>
+      </c>
+      <c r="H83" t="s">
+        <v>34</v>
       </c>
       <c r="J83" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10">
-      <c r="B84" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" s="15" customFormat="1">
-      <c r="A85" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="D85" s="16"/>
-      <c r="E85" s="16"/>
-      <c r="F85" s="16"/>
-      <c r="I85" s="16"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" s="15" customFormat="1">
+      <c r="A84" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D84" s="16"/>
+      <c r="E84" s="16"/>
+      <c r="F84" s="16"/>
+      <c r="I84" s="16"/>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="B85" t="s">
+        <v>69</v>
+      </c>
+      <c r="J85" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="86" spans="1:10">
       <c r="B86" t="s">
-        <v>94</v>
-      </c>
-      <c r="G86" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="J86" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="B87" t="s">
-        <v>98</v>
-      </c>
-      <c r="G87" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="J87" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="B88" t="s">
-        <v>101</v>
-      </c>
-      <c r="G88" t="s">
-        <v>100</v>
-      </c>
-      <c r="J88" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10">
-      <c r="B89" t="s">
-        <v>104</v>
-      </c>
-      <c r="G89" t="s">
-        <v>103</v>
-      </c>
-      <c r="J89" t="s">
-        <v>102</v>
-      </c>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" s="15" customFormat="1">
+      <c r="A89" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D89" s="16"/>
+      <c r="E89" s="16"/>
+      <c r="F89" s="16"/>
+      <c r="I89" s="16"/>
     </row>
     <row r="90" spans="1:10">
       <c r="B90" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="G90" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="J90" t="s">
-        <v>105</v>
+        <v>57</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="B91" t="s">
+        <v>98</v>
+      </c>
+      <c r="G91" t="s">
+        <v>97</v>
+      </c>
+      <c r="J91" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="B92" t="s">
+        <v>101</v>
+      </c>
+      <c r="G92" t="s">
+        <v>100</v>
+      </c>
+      <c r="J92" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="B93" t="s">
+        <v>104</v>
+      </c>
+      <c r="G93" t="s">
+        <v>103</v>
+      </c>
+      <c r="J93" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="B94" t="s">
+        <v>106</v>
+      </c>
+      <c r="G94" t="s">
+        <v>110</v>
+      </c>
+      <c r="J94" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="B95" t="s">
         <v>108</v>
       </c>
-      <c r="G91" t="s">
+      <c r="G95" t="s">
         <v>109</v>
       </c>
-      <c r="J91" t="s">
+      <c r="J95" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="92" spans="1:10" s="24" customFormat="1">
-      <c r="A92" s="24" t="s">
+    <row r="96" spans="1:10" s="24" customFormat="1">
+      <c r="A96" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="D92" s="25"/>
-      <c r="E92" s="25"/>
-      <c r="F92" s="25"/>
-      <c r="I92" s="25"/>
-    </row>
-    <row r="93" spans="1:10">
-      <c r="J93" s="1" t="s">
+      <c r="D96" s="25"/>
+      <c r="E96" s="25"/>
+      <c r="F96" s="25"/>
+      <c r="I96" s="25"/>
+    </row>
+    <row r="97" spans="10:10">
+      <c r="J97" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
-      <c r="J94" t="s">
+    <row r="98" spans="10:10">
+      <c r="J98" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2713,8 +2764,8 @@
     <hyperlink ref="J11" r:id="rId1" xr:uid="{E14B3450-24AC-4CFD-8025-A3383681EF6E}"/>
     <hyperlink ref="J13" r:id="rId2" xr:uid="{E04BDA5B-F93E-430F-91E8-9DFA7F84D927}"/>
     <hyperlink ref="J35" r:id="rId3" xr:uid="{F64AADB2-C73B-49A3-9212-3983BBEF9380}"/>
-    <hyperlink ref="J93" r:id="rId4" xr:uid="{A2FD99F1-6002-4AF5-B586-6D2A968B5797}"/>
-    <hyperlink ref="J62" r:id="rId5" xr:uid="{0A94D00C-75FB-49FF-8ECE-3641A5A57E0E}"/>
+    <hyperlink ref="J97" r:id="rId4" xr:uid="{A2FD99F1-6002-4AF5-B586-6D2A968B5797}"/>
+    <hyperlink ref="J66" r:id="rId5" xr:uid="{0A94D00C-75FB-49FF-8ECE-3641A5A57E0E}"/>
     <hyperlink ref="J20" r:id="rId6" xr:uid="{E56CD8F7-0A95-4862-924E-AD4163C0BE86}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>